<commit_message>
Added no-token api route and fixed baseURL
the /no-token route from account api applies to the login page only. If there's no token, the user can proceed; otherwise, they are redirected back to the homepage.

also fixed the issue with axios.default.baseURL. This allows for components to not include the entire route when calling to the backend server.
</commit_message>
<xml_diff>
--- a/documentation/environment.xlsx
+++ b/documentation/environment.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/82c9ca36d704f7f3/Documents/GitHub/adventure_time_academy/documentation/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Public\Downloads\adventure_time_academy\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="28" documentId="8_{343A90F2-12DB-4058-B9C4-36AE81AABCF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{ED7D575E-76EB-4207-9F10-94ADB7E1B25B}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0042761B-5BE4-4E6C-A608-4292609E830E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{C00B0261-B5E8-41DD-9D58-BD162CA62124}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{C00B0261-B5E8-41DD-9D58-BD162CA62124}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="29">
   <si>
     <t>Backend</t>
   </si>
@@ -92,12 +92,6 @@
     <t>http://localhost:</t>
   </si>
   <si>
-    <t>http://localhost:8080</t>
-  </si>
-  <si>
-    <t>Test</t>
-  </si>
-  <si>
     <t>Production</t>
   </si>
   <si>
@@ -116,7 +110,19 @@
     <t>localhost</t>
   </si>
   <si>
-    <t>http://localhost:8081/api</t>
+    <t>Development</t>
+  </si>
+  <si>
+    <t>http://localhost:5000</t>
+  </si>
+  <si>
+    <t>http://localhost:9080</t>
+  </si>
+  <si>
+    <t>NODE_ENV</t>
+  </si>
+  <si>
+    <t>development</t>
   </si>
 </sst>
 </file>
@@ -187,11 +193,11 @@
     </border>
     <border>
       <left/>
-      <right style="thin">
+      <right/>
+      <top/>
+      <bottom style="thin">
         <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -199,22 +205,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -222,6 +219,12 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -558,15 +561,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7569776-A18F-4387-97BF-46244A4B9686}">
-  <dimension ref="A1:K9"/>
+  <dimension ref="A1:L9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="39.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="22" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="54.7109375" bestFit="1" customWidth="1"/>
@@ -574,25 +577,26 @@
     <col min="7" max="7" width="23.7109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="36.5703125" bestFit="1" customWidth="1"/>
     <col min="9" max="10" width="17.7109375" customWidth="1"/>
-    <col min="11" max="11" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="19.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
       <c r="K1" s="6"/>
+      <c r="L1" s="6"/>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
       <c r="B2" s="1" t="s">
         <v>1</v>
@@ -624,45 +628,51 @@
       <c r="K2" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="L2" s="1" t="s">
+        <v>27</v>
+      </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="B3" s="4" t="s">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="4">
+      <c r="C3" s="3">
         <v>3306</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="F3" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="G3" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="H3" s="4" t="s">
+      <c r="H3" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="I3" s="4">
-        <v>8081</v>
-      </c>
-      <c r="J3" s="4" t="s">
+      <c r="I3" s="3">
+        <v>5000</v>
+      </c>
+      <c r="J3" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="K3" s="4" t="s">
+      <c r="K3" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
         <v>18</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="7" t="s">
-        <v>20</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
@@ -674,57 +684,55 @@
       <c r="I4" s="2"/>
       <c r="J4" s="2"/>
       <c r="K4" s="2"/>
+      <c r="L4" s="2"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="7"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
       <c r="B7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C7" s="1" t="s">
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" s="3">
+        <v>9080</v>
+      </c>
+      <c r="D8" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D7" s="1" t="s">
-        <v>24</v>
-      </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="B8" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="C8" s="4">
-        <v>8080</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A1:K1"/>
     <mergeCell ref="A6:D6"/>
+    <mergeCell ref="A1:L1"/>
   </mergeCells>
-  <hyperlinks>
-    <hyperlink ref="B8" r:id="rId1" xr:uid="{2AADE9A2-E723-420E-9114-30F3A433C58F}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>